<commit_message>
Bài 18 : Excel VSTO - API
</commit_message>
<xml_diff>
--- a/ExcelWorkbook/ExcelWorkbook.xlsx
+++ b/ExcelWorkbook/ExcelWorkbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28304"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28306"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kysudo\source\repos\BIMSoftVN\K008\ExcelWorkbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C6DDBEF-B76C-4907-A206-26AF4461B2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455519C8-BA80-4556-B6C9-41C658A1EED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4AB6F734-EEB6-4FDD-95EB-EC5BA8E33ED8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ngày</t>
   </si>
@@ -51,13 +51,22 @@
   </si>
   <si>
     <t>Thời tiết</t>
+  </si>
+  <si>
+    <t>Thành phố</t>
+  </si>
+  <si>
+    <t>Hình Ảnh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +82,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -115,9 +138,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,35 +479,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5832BAC-AD37-4A5A-A008-FCE2B1613951}">
-  <dimension ref="A1:E1"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="5" customWidth="1"/>
+    <col min="3" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>